<commit_message>
fixed mistake in population sector where conveyors were initialized backwards
</commit_message>
<xml_diff>
--- a/Data Processing/Age Specific Population Data.xlsx
+++ b/Data Processing/Age Specific Population Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bschoenberg/code/WorldTrans/Frida/Data Processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17AC6723-374D-F148-BDDF-FE0D5F8EDEDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3F7B535-B804-144F-8646-F0FDCC5F215C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UN Data" sheetId="1" r:id="rId1"/>
@@ -69017,8 +69017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E100"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E100"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -69045,14 +69045,14 @@
         <v>492</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
         <v>490</v>
       </c>
       <c r="D2" t="str">
         <f t="shared" ref="D2:D65" si="0">_xlfn.CONCAT(A2,B2,C2)</f>
-        <v>Population.Aged 1 to 20 in 1980[1]</v>
+        <v>Population.Aged 1 to 20 in 1980[19]</v>
       </c>
       <c r="E2">
         <f>'UN Data'!B3</f>
@@ -69064,15 +69064,15 @@
         <v>492</v>
       </c>
       <c r="B3">
-        <f>B2+1</f>
-        <v>2</v>
+        <f>B2-1</f>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
         <v>490</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 1 to 20 in 1980[2]</v>
+        <v>Population.Aged 1 to 20 in 1980[18]</v>
       </c>
       <c r="E3">
         <f>'UN Data'!B4</f>
@@ -69084,15 +69084,15 @@
         <v>492</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:B20" si="1">B3+1</f>
-        <v>3</v>
+        <f t="shared" ref="B4:B20" si="1">B3-1</f>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
         <v>490</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 1 to 20 in 1980[3]</v>
+        <v>Population.Aged 1 to 20 in 1980[17]</v>
       </c>
       <c r="E4">
         <f>'UN Data'!B5</f>
@@ -69105,14 +69105,14 @@
       </c>
       <c r="B5">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
         <v>490</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 1 to 20 in 1980[4]</v>
+        <v>Population.Aged 1 to 20 in 1980[16]</v>
       </c>
       <c r="E5">
         <f>'UN Data'!B6</f>
@@ -69125,14 +69125,14 @@
       </c>
       <c r="B6">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
         <v>490</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 1 to 20 in 1980[5]</v>
+        <v>Population.Aged 1 to 20 in 1980[15]</v>
       </c>
       <c r="E6">
         <f>'UN Data'!B7</f>
@@ -69145,14 +69145,14 @@
       </c>
       <c r="B7">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
         <v>490</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 1 to 20 in 1980[6]</v>
+        <v>Population.Aged 1 to 20 in 1980[14]</v>
       </c>
       <c r="E7">
         <f>'UN Data'!B8</f>
@@ -69165,14 +69165,14 @@
       </c>
       <c r="B8">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
         <v>490</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 1 to 20 in 1980[7]</v>
+        <v>Population.Aged 1 to 20 in 1980[13]</v>
       </c>
       <c r="E8">
         <f>'UN Data'!B9</f>
@@ -69185,14 +69185,14 @@
       </c>
       <c r="B9">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
         <v>490</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 1 to 20 in 1980[8]</v>
+        <v>Population.Aged 1 to 20 in 1980[12]</v>
       </c>
       <c r="E9">
         <f>'UN Data'!B10</f>
@@ -69205,14 +69205,14 @@
       </c>
       <c r="B10">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
         <v>490</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 1 to 20 in 1980[9]</v>
+        <v>Population.Aged 1 to 20 in 1980[11]</v>
       </c>
       <c r="E10">
         <f>'UN Data'!B11</f>
@@ -69245,14 +69245,14 @@
       </c>
       <c r="B12">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
         <v>490</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 1 to 20 in 1980[11]</v>
+        <v>Population.Aged 1 to 20 in 1980[9]</v>
       </c>
       <c r="E12">
         <f>'UN Data'!B13</f>
@@ -69265,14 +69265,14 @@
       </c>
       <c r="B13">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C13" t="s">
         <v>490</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 1 to 20 in 1980[12]</v>
+        <v>Population.Aged 1 to 20 in 1980[8]</v>
       </c>
       <c r="E13">
         <f>'UN Data'!B14</f>
@@ -69285,14 +69285,14 @@
       </c>
       <c r="B14">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C14" t="s">
         <v>490</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 1 to 20 in 1980[13]</v>
+        <v>Population.Aged 1 to 20 in 1980[7]</v>
       </c>
       <c r="E14">
         <f>'UN Data'!B15</f>
@@ -69305,14 +69305,14 @@
       </c>
       <c r="B15">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C15" t="s">
         <v>490</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 1 to 20 in 1980[14]</v>
+        <v>Population.Aged 1 to 20 in 1980[6]</v>
       </c>
       <c r="E15">
         <f>'UN Data'!B16</f>
@@ -69325,14 +69325,14 @@
       </c>
       <c r="B16">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C16" t="s">
         <v>490</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 1 to 20 in 1980[15]</v>
+        <v>Population.Aged 1 to 20 in 1980[5]</v>
       </c>
       <c r="E16">
         <f>'UN Data'!B17</f>
@@ -69345,14 +69345,14 @@
       </c>
       <c r="B17">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C17" t="s">
         <v>490</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 1 to 20 in 1980[16]</v>
+        <v>Population.Aged 1 to 20 in 1980[4]</v>
       </c>
       <c r="E17">
         <f>'UN Data'!B18</f>
@@ -69365,14 +69365,14 @@
       </c>
       <c r="B18">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C18" t="s">
         <v>490</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 1 to 20 in 1980[17]</v>
+        <v>Population.Aged 1 to 20 in 1980[3]</v>
       </c>
       <c r="E18">
         <f>'UN Data'!B19</f>
@@ -69385,14 +69385,14 @@
       </c>
       <c r="B19">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C19" t="s">
         <v>490</v>
       </c>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 1 to 20 in 1980[18]</v>
+        <v>Population.Aged 1 to 20 in 1980[2]</v>
       </c>
       <c r="E19">
         <f>'UN Data'!B20</f>
@@ -69405,14 +69405,14 @@
       </c>
       <c r="B20">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="C20" t="s">
         <v>490</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 1 to 20 in 1980[19]</v>
+        <v>Population.Aged 1 to 20 in 1980[1]</v>
       </c>
       <c r="E20">
         <f>'UN Data'!B21</f>
@@ -69424,14 +69424,14 @@
         <v>493</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C21" t="s">
         <v>490</v>
       </c>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 20 to 40 in 1980[1]</v>
+        <v>Population.Aged 20 to 40 in 1980[20]</v>
       </c>
       <c r="E21">
         <f>'UN Data'!B22</f>
@@ -69443,15 +69443,15 @@
         <v>493</v>
       </c>
       <c r="B22">
-        <f>B21+1</f>
-        <v>2</v>
+        <f>B21-1</f>
+        <v>19</v>
       </c>
       <c r="C22" t="s">
         <v>490</v>
       </c>
       <c r="D22" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 20 to 40 in 1980[2]</v>
+        <v>Population.Aged 20 to 40 in 1980[19]</v>
       </c>
       <c r="E22">
         <f>'UN Data'!B23</f>
@@ -69463,15 +69463,15 @@
         <v>493</v>
       </c>
       <c r="B23">
-        <f t="shared" ref="B23:B40" si="2">B22+1</f>
-        <v>3</v>
+        <f t="shared" ref="B23:B40" si="2">B22-1</f>
+        <v>18</v>
       </c>
       <c r="C23" t="s">
         <v>490</v>
       </c>
       <c r="D23" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 20 to 40 in 1980[3]</v>
+        <v>Population.Aged 20 to 40 in 1980[18]</v>
       </c>
       <c r="E23">
         <f>'UN Data'!B24</f>
@@ -69484,14 +69484,14 @@
       </c>
       <c r="B24">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C24" t="s">
         <v>490</v>
       </c>
       <c r="D24" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 20 to 40 in 1980[4]</v>
+        <v>Population.Aged 20 to 40 in 1980[17]</v>
       </c>
       <c r="E24">
         <f>'UN Data'!B25</f>
@@ -69504,14 +69504,14 @@
       </c>
       <c r="B25">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C25" t="s">
         <v>490</v>
       </c>
       <c r="D25" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 20 to 40 in 1980[5]</v>
+        <v>Population.Aged 20 to 40 in 1980[16]</v>
       </c>
       <c r="E25">
         <f>'UN Data'!B26</f>
@@ -69524,14 +69524,14 @@
       </c>
       <c r="B26">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C26" t="s">
         <v>490</v>
       </c>
       <c r="D26" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 20 to 40 in 1980[6]</v>
+        <v>Population.Aged 20 to 40 in 1980[15]</v>
       </c>
       <c r="E26">
         <f>'UN Data'!B27</f>
@@ -69544,14 +69544,14 @@
       </c>
       <c r="B27">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C27" t="s">
         <v>490</v>
       </c>
       <c r="D27" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 20 to 40 in 1980[7]</v>
+        <v>Population.Aged 20 to 40 in 1980[14]</v>
       </c>
       <c r="E27">
         <f>'UN Data'!B28</f>
@@ -69564,14 +69564,14 @@
       </c>
       <c r="B28">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C28" t="s">
         <v>490</v>
       </c>
       <c r="D28" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 20 to 40 in 1980[8]</v>
+        <v>Population.Aged 20 to 40 in 1980[13]</v>
       </c>
       <c r="E28">
         <f>'UN Data'!B29</f>
@@ -69584,14 +69584,14 @@
       </c>
       <c r="B29">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C29" t="s">
         <v>490</v>
       </c>
       <c r="D29" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 20 to 40 in 1980[9]</v>
+        <v>Population.Aged 20 to 40 in 1980[12]</v>
       </c>
       <c r="E29">
         <f>'UN Data'!B30</f>
@@ -69604,14 +69604,14 @@
       </c>
       <c r="B30">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C30" t="s">
         <v>490</v>
       </c>
       <c r="D30" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 20 to 40 in 1980[10]</v>
+        <v>Population.Aged 20 to 40 in 1980[11]</v>
       </c>
       <c r="E30">
         <f>'UN Data'!B31</f>
@@ -69624,14 +69624,14 @@
       </c>
       <c r="B31">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C31" t="s">
         <v>490</v>
       </c>
       <c r="D31" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 20 to 40 in 1980[11]</v>
+        <v>Population.Aged 20 to 40 in 1980[10]</v>
       </c>
       <c r="E31">
         <f>'UN Data'!B32</f>
@@ -69644,14 +69644,14 @@
       </c>
       <c r="B32">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C32" t="s">
         <v>490</v>
       </c>
       <c r="D32" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 20 to 40 in 1980[12]</v>
+        <v>Population.Aged 20 to 40 in 1980[9]</v>
       </c>
       <c r="E32">
         <f>'UN Data'!B33</f>
@@ -69664,14 +69664,14 @@
       </c>
       <c r="B33">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C33" t="s">
         <v>490</v>
       </c>
       <c r="D33" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 20 to 40 in 1980[13]</v>
+        <v>Population.Aged 20 to 40 in 1980[8]</v>
       </c>
       <c r="E33">
         <f>'UN Data'!B34</f>
@@ -69684,14 +69684,14 @@
       </c>
       <c r="B34">
         <f t="shared" si="2"/>
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C34" t="s">
         <v>490</v>
       </c>
       <c r="D34" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 20 to 40 in 1980[14]</v>
+        <v>Population.Aged 20 to 40 in 1980[7]</v>
       </c>
       <c r="E34">
         <f>'UN Data'!B35</f>
@@ -69704,14 +69704,14 @@
       </c>
       <c r="B35">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C35" t="s">
         <v>490</v>
       </c>
       <c r="D35" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 20 to 40 in 1980[15]</v>
+        <v>Population.Aged 20 to 40 in 1980[6]</v>
       </c>
       <c r="E35">
         <f>'UN Data'!B36</f>
@@ -69724,14 +69724,14 @@
       </c>
       <c r="B36">
         <f t="shared" si="2"/>
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C36" t="s">
         <v>490</v>
       </c>
       <c r="D36" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 20 to 40 in 1980[16]</v>
+        <v>Population.Aged 20 to 40 in 1980[5]</v>
       </c>
       <c r="E36">
         <f>'UN Data'!B37</f>
@@ -69744,14 +69744,14 @@
       </c>
       <c r="B37">
         <f t="shared" si="2"/>
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C37" t="s">
         <v>490</v>
       </c>
       <c r="D37" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 20 to 40 in 1980[17]</v>
+        <v>Population.Aged 20 to 40 in 1980[4]</v>
       </c>
       <c r="E37">
         <f>'UN Data'!B38</f>
@@ -69764,14 +69764,14 @@
       </c>
       <c r="B38">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="C38" t="s">
         <v>490</v>
       </c>
       <c r="D38" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 20 to 40 in 1980[18]</v>
+        <v>Population.Aged 20 to 40 in 1980[3]</v>
       </c>
       <c r="E38">
         <f>'UN Data'!B39</f>
@@ -69784,14 +69784,14 @@
       </c>
       <c r="B39">
         <f t="shared" si="2"/>
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="C39" t="s">
         <v>490</v>
       </c>
       <c r="D39" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 20 to 40 in 1980[19]</v>
+        <v>Population.Aged 20 to 40 in 1980[2]</v>
       </c>
       <c r="E39">
         <f>'UN Data'!B40</f>
@@ -69804,14 +69804,14 @@
       </c>
       <c r="B40">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C40" t="s">
         <v>490</v>
       </c>
       <c r="D40" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 20 to 40 in 1980[20]</v>
+        <v>Population.Aged 20 to 40 in 1980[1]</v>
       </c>
       <c r="E40">
         <f>'UN Data'!B41</f>
@@ -69824,14 +69824,14 @@
       </c>
       <c r="B41">
         <f>B21</f>
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C41" t="s">
         <v>490</v>
       </c>
       <c r="D41" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 40 to 60 in 1980[1]</v>
+        <v>Population.Aged 40 to 60 in 1980[20]</v>
       </c>
       <c r="E41">
         <f>'UN Data'!B42</f>
@@ -69844,14 +69844,14 @@
       </c>
       <c r="B42">
         <f t="shared" ref="B42:B100" si="3">B22</f>
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C42" t="s">
         <v>490</v>
       </c>
       <c r="D42" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 40 to 60 in 1980[2]</v>
+        <v>Population.Aged 40 to 60 in 1980[19]</v>
       </c>
       <c r="E42">
         <f>'UN Data'!B43</f>
@@ -69864,14 +69864,14 @@
       </c>
       <c r="B43">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C43" t="s">
         <v>490</v>
       </c>
       <c r="D43" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 40 to 60 in 1980[3]</v>
+        <v>Population.Aged 40 to 60 in 1980[18]</v>
       </c>
       <c r="E43">
         <f>'UN Data'!B44</f>
@@ -69884,14 +69884,14 @@
       </c>
       <c r="B44">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C44" t="s">
         <v>490</v>
       </c>
       <c r="D44" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 40 to 60 in 1980[4]</v>
+        <v>Population.Aged 40 to 60 in 1980[17]</v>
       </c>
       <c r="E44">
         <f>'UN Data'!B45</f>
@@ -69904,14 +69904,14 @@
       </c>
       <c r="B45">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C45" t="s">
         <v>490</v>
       </c>
       <c r="D45" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 40 to 60 in 1980[5]</v>
+        <v>Population.Aged 40 to 60 in 1980[16]</v>
       </c>
       <c r="E45">
         <f>'UN Data'!B46</f>
@@ -69924,14 +69924,14 @@
       </c>
       <c r="B46">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C46" t="s">
         <v>490</v>
       </c>
       <c r="D46" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 40 to 60 in 1980[6]</v>
+        <v>Population.Aged 40 to 60 in 1980[15]</v>
       </c>
       <c r="E46">
         <f>'UN Data'!B47</f>
@@ -69944,14 +69944,14 @@
       </c>
       <c r="B47">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C47" t="s">
         <v>490</v>
       </c>
       <c r="D47" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 40 to 60 in 1980[7]</v>
+        <v>Population.Aged 40 to 60 in 1980[14]</v>
       </c>
       <c r="E47">
         <f>'UN Data'!B48</f>
@@ -69964,14 +69964,14 @@
       </c>
       <c r="B48">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C48" t="s">
         <v>490</v>
       </c>
       <c r="D48" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 40 to 60 in 1980[8]</v>
+        <v>Population.Aged 40 to 60 in 1980[13]</v>
       </c>
       <c r="E48">
         <f>'UN Data'!B49</f>
@@ -69984,14 +69984,14 @@
       </c>
       <c r="B49">
         <f t="shared" si="3"/>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C49" t="s">
         <v>490</v>
       </c>
       <c r="D49" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 40 to 60 in 1980[9]</v>
+        <v>Population.Aged 40 to 60 in 1980[12]</v>
       </c>
       <c r="E49">
         <f>'UN Data'!B50</f>
@@ -70004,14 +70004,14 @@
       </c>
       <c r="B50">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C50" t="s">
         <v>490</v>
       </c>
       <c r="D50" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 40 to 60 in 1980[10]</v>
+        <v>Population.Aged 40 to 60 in 1980[11]</v>
       </c>
       <c r="E50">
         <f>'UN Data'!B51</f>
@@ -70024,14 +70024,14 @@
       </c>
       <c r="B51">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C51" t="s">
         <v>490</v>
       </c>
       <c r="D51" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 40 to 60 in 1980[11]</v>
+        <v>Population.Aged 40 to 60 in 1980[10]</v>
       </c>
       <c r="E51">
         <f>'UN Data'!B52</f>
@@ -70044,14 +70044,14 @@
       </c>
       <c r="B52">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C52" t="s">
         <v>490</v>
       </c>
       <c r="D52" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 40 to 60 in 1980[12]</v>
+        <v>Population.Aged 40 to 60 in 1980[9]</v>
       </c>
       <c r="E52">
         <f>'UN Data'!B53</f>
@@ -70064,14 +70064,14 @@
       </c>
       <c r="B53">
         <f t="shared" si="3"/>
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C53" t="s">
         <v>490</v>
       </c>
       <c r="D53" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 40 to 60 in 1980[13]</v>
+        <v>Population.Aged 40 to 60 in 1980[8]</v>
       </c>
       <c r="E53">
         <f>'UN Data'!B54</f>
@@ -70084,14 +70084,14 @@
       </c>
       <c r="B54">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C54" t="s">
         <v>490</v>
       </c>
       <c r="D54" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 40 to 60 in 1980[14]</v>
+        <v>Population.Aged 40 to 60 in 1980[7]</v>
       </c>
       <c r="E54">
         <f>'UN Data'!B55</f>
@@ -70104,14 +70104,14 @@
       </c>
       <c r="B55">
         <f t="shared" si="3"/>
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C55" t="s">
         <v>490</v>
       </c>
       <c r="D55" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 40 to 60 in 1980[15]</v>
+        <v>Population.Aged 40 to 60 in 1980[6]</v>
       </c>
       <c r="E55">
         <f>'UN Data'!B56</f>
@@ -70124,14 +70124,14 @@
       </c>
       <c r="B56">
         <f t="shared" si="3"/>
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C56" t="s">
         <v>490</v>
       </c>
       <c r="D56" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 40 to 60 in 1980[16]</v>
+        <v>Population.Aged 40 to 60 in 1980[5]</v>
       </c>
       <c r="E56">
         <f>'UN Data'!B57</f>
@@ -70144,14 +70144,14 @@
       </c>
       <c r="B57">
         <f t="shared" si="3"/>
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C57" t="s">
         <v>490</v>
       </c>
       <c r="D57" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 40 to 60 in 1980[17]</v>
+        <v>Population.Aged 40 to 60 in 1980[4]</v>
       </c>
       <c r="E57">
         <f>'UN Data'!B58</f>
@@ -70164,14 +70164,14 @@
       </c>
       <c r="B58">
         <f t="shared" si="3"/>
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="C58" t="s">
         <v>490</v>
       </c>
       <c r="D58" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 40 to 60 in 1980[18]</v>
+        <v>Population.Aged 40 to 60 in 1980[3]</v>
       </c>
       <c r="E58">
         <f>'UN Data'!B59</f>
@@ -70184,14 +70184,14 @@
       </c>
       <c r="B59">
         <f t="shared" si="3"/>
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="C59" t="s">
         <v>490</v>
       </c>
       <c r="D59" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 40 to 60 in 1980[19]</v>
+        <v>Population.Aged 40 to 60 in 1980[2]</v>
       </c>
       <c r="E59">
         <f>'UN Data'!B60</f>
@@ -70204,14 +70204,14 @@
       </c>
       <c r="B60">
         <f t="shared" si="3"/>
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C60" t="s">
         <v>490</v>
       </c>
       <c r="D60" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 40 to 60 in 1980[20]</v>
+        <v>Population.Aged 40 to 60 in 1980[1]</v>
       </c>
       <c r="E60">
         <f>'UN Data'!B61</f>
@@ -70224,14 +70224,14 @@
       </c>
       <c r="B61">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C61" t="s">
         <v>490</v>
       </c>
       <c r="D61" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 60 to 80 in 1980[1]</v>
+        <v>Population.Aged 60 to 80 in 1980[20]</v>
       </c>
       <c r="E61">
         <f>'UN Data'!B62</f>
@@ -70244,14 +70244,14 @@
       </c>
       <c r="B62">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C62" t="s">
         <v>490</v>
       </c>
       <c r="D62" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 60 to 80 in 1980[2]</v>
+        <v>Population.Aged 60 to 80 in 1980[19]</v>
       </c>
       <c r="E62">
         <f>'UN Data'!B63</f>
@@ -70264,14 +70264,14 @@
       </c>
       <c r="B63">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C63" t="s">
         <v>490</v>
       </c>
       <c r="D63" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 60 to 80 in 1980[3]</v>
+        <v>Population.Aged 60 to 80 in 1980[18]</v>
       </c>
       <c r="E63">
         <f>'UN Data'!B64</f>
@@ -70284,14 +70284,14 @@
       </c>
       <c r="B64">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C64" t="s">
         <v>490</v>
       </c>
       <c r="D64" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 60 to 80 in 1980[4]</v>
+        <v>Population.Aged 60 to 80 in 1980[17]</v>
       </c>
       <c r="E64">
         <f>'UN Data'!B65</f>
@@ -70304,14 +70304,14 @@
       </c>
       <c r="B65">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C65" t="s">
         <v>490</v>
       </c>
       <c r="D65" t="str">
         <f t="shared" si="0"/>
-        <v>Population.Aged 60 to 80 in 1980[5]</v>
+        <v>Population.Aged 60 to 80 in 1980[16]</v>
       </c>
       <c r="E65">
         <f>'UN Data'!B66</f>
@@ -70324,14 +70324,14 @@
       </c>
       <c r="B66">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C66" t="s">
         <v>490</v>
       </c>
       <c r="D66" t="str">
         <f t="shared" ref="D66:D100" si="4">_xlfn.CONCAT(A66,B66,C66)</f>
-        <v>Population.Aged 60 to 80 in 1980[6]</v>
+        <v>Population.Aged 60 to 80 in 1980[15]</v>
       </c>
       <c r="E66">
         <f>'UN Data'!B67</f>
@@ -70344,14 +70344,14 @@
       </c>
       <c r="B67">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C67" t="s">
         <v>490</v>
       </c>
       <c r="D67" t="str">
         <f t="shared" si="4"/>
-        <v>Population.Aged 60 to 80 in 1980[7]</v>
+        <v>Population.Aged 60 to 80 in 1980[14]</v>
       </c>
       <c r="E67">
         <f>'UN Data'!B68</f>
@@ -70364,14 +70364,14 @@
       </c>
       <c r="B68">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C68" t="s">
         <v>490</v>
       </c>
       <c r="D68" t="str">
         <f t="shared" si="4"/>
-        <v>Population.Aged 60 to 80 in 1980[8]</v>
+        <v>Population.Aged 60 to 80 in 1980[13]</v>
       </c>
       <c r="E68">
         <f>'UN Data'!B69</f>
@@ -70384,14 +70384,14 @@
       </c>
       <c r="B69">
         <f t="shared" si="3"/>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C69" t="s">
         <v>490</v>
       </c>
       <c r="D69" t="str">
         <f t="shared" si="4"/>
-        <v>Population.Aged 60 to 80 in 1980[9]</v>
+        <v>Population.Aged 60 to 80 in 1980[12]</v>
       </c>
       <c r="E69">
         <f>'UN Data'!B70</f>
@@ -70404,14 +70404,14 @@
       </c>
       <c r="B70">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C70" t="s">
         <v>490</v>
       </c>
       <c r="D70" t="str">
         <f t="shared" si="4"/>
-        <v>Population.Aged 60 to 80 in 1980[10]</v>
+        <v>Population.Aged 60 to 80 in 1980[11]</v>
       </c>
       <c r="E70">
         <f>'UN Data'!B71</f>
@@ -70424,14 +70424,14 @@
       </c>
       <c r="B71">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C71" t="s">
         <v>490</v>
       </c>
       <c r="D71" t="str">
         <f t="shared" si="4"/>
-        <v>Population.Aged 60 to 80 in 1980[11]</v>
+        <v>Population.Aged 60 to 80 in 1980[10]</v>
       </c>
       <c r="E71">
         <f>'UN Data'!B72</f>
@@ -70444,14 +70444,14 @@
       </c>
       <c r="B72">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C72" t="s">
         <v>490</v>
       </c>
       <c r="D72" t="str">
         <f t="shared" si="4"/>
-        <v>Population.Aged 60 to 80 in 1980[12]</v>
+        <v>Population.Aged 60 to 80 in 1980[9]</v>
       </c>
       <c r="E72">
         <f>'UN Data'!B73</f>
@@ -70464,14 +70464,14 @@
       </c>
       <c r="B73">
         <f t="shared" si="3"/>
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C73" t="s">
         <v>490</v>
       </c>
       <c r="D73" t="str">
         <f t="shared" si="4"/>
-        <v>Population.Aged 60 to 80 in 1980[13]</v>
+        <v>Population.Aged 60 to 80 in 1980[8]</v>
       </c>
       <c r="E73">
         <f>'UN Data'!B74</f>
@@ -70484,14 +70484,14 @@
       </c>
       <c r="B74">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C74" t="s">
         <v>490</v>
       </c>
       <c r="D74" t="str">
         <f t="shared" si="4"/>
-        <v>Population.Aged 60 to 80 in 1980[14]</v>
+        <v>Population.Aged 60 to 80 in 1980[7]</v>
       </c>
       <c r="E74">
         <f>'UN Data'!B75</f>
@@ -70504,14 +70504,14 @@
       </c>
       <c r="B75">
         <f t="shared" si="3"/>
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C75" t="s">
         <v>490</v>
       </c>
       <c r="D75" t="str">
         <f t="shared" si="4"/>
-        <v>Population.Aged 60 to 80 in 1980[15]</v>
+        <v>Population.Aged 60 to 80 in 1980[6]</v>
       </c>
       <c r="E75">
         <f>'UN Data'!B76</f>
@@ -70524,14 +70524,14 @@
       </c>
       <c r="B76">
         <f t="shared" si="3"/>
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C76" t="s">
         <v>490</v>
       </c>
       <c r="D76" t="str">
         <f t="shared" si="4"/>
-        <v>Population.Aged 60 to 80 in 1980[16]</v>
+        <v>Population.Aged 60 to 80 in 1980[5]</v>
       </c>
       <c r="E76">
         <f>'UN Data'!B77</f>
@@ -70544,14 +70544,14 @@
       </c>
       <c r="B77">
         <f t="shared" si="3"/>
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C77" t="s">
         <v>490</v>
       </c>
       <c r="D77" t="str">
         <f t="shared" si="4"/>
-        <v>Population.Aged 60 to 80 in 1980[17]</v>
+        <v>Population.Aged 60 to 80 in 1980[4]</v>
       </c>
       <c r="E77">
         <f>'UN Data'!B78</f>
@@ -70564,14 +70564,14 @@
       </c>
       <c r="B78">
         <f t="shared" si="3"/>
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="C78" t="s">
         <v>490</v>
       </c>
       <c r="D78" t="str">
         <f t="shared" si="4"/>
-        <v>Population.Aged 60 to 80 in 1980[18]</v>
+        <v>Population.Aged 60 to 80 in 1980[3]</v>
       </c>
       <c r="E78">
         <f>'UN Data'!B79</f>
@@ -70584,14 +70584,14 @@
       </c>
       <c r="B79">
         <f t="shared" si="3"/>
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="C79" t="s">
         <v>490</v>
       </c>
       <c r="D79" t="str">
         <f t="shared" si="4"/>
-        <v>Population.Aged 60 to 80 in 1980[19]</v>
+        <v>Population.Aged 60 to 80 in 1980[2]</v>
       </c>
       <c r="E79">
         <f>'UN Data'!B80</f>
@@ -70604,14 +70604,14 @@
       </c>
       <c r="B80">
         <f t="shared" si="3"/>
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C80" t="s">
         <v>490</v>
       </c>
       <c r="D80" t="str">
         <f t="shared" si="4"/>
-        <v>Population.Aged 60 to 80 in 1980[20]</v>
+        <v>Population.Aged 60 to 80 in 1980[1]</v>
       </c>
       <c r="E80">
         <f>'UN Data'!B81</f>
@@ -70624,14 +70624,14 @@
       </c>
       <c r="B81">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C81" t="s">
         <v>490</v>
       </c>
       <c r="D81" t="str">
         <f t="shared" si="4"/>
-        <v>Population.Aged Over 80 in 1980[1]</v>
+        <v>Population.Aged Over 80 in 1980[20]</v>
       </c>
       <c r="E81">
         <f>'UN Data'!B82</f>
@@ -70644,14 +70644,14 @@
       </c>
       <c r="B82">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C82" t="s">
         <v>490</v>
       </c>
       <c r="D82" t="str">
         <f t="shared" si="4"/>
-        <v>Population.Aged Over 80 in 1980[2]</v>
+        <v>Population.Aged Over 80 in 1980[19]</v>
       </c>
       <c r="E82">
         <f>'UN Data'!B83</f>
@@ -70664,14 +70664,14 @@
       </c>
       <c r="B83">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C83" t="s">
         <v>490</v>
       </c>
       <c r="D83" t="str">
         <f t="shared" si="4"/>
-        <v>Population.Aged Over 80 in 1980[3]</v>
+        <v>Population.Aged Over 80 in 1980[18]</v>
       </c>
       <c r="E83">
         <f>'UN Data'!B84</f>
@@ -70684,14 +70684,14 @@
       </c>
       <c r="B84">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C84" t="s">
         <v>490</v>
       </c>
       <c r="D84" t="str">
         <f t="shared" si="4"/>
-        <v>Population.Aged Over 80 in 1980[4]</v>
+        <v>Population.Aged Over 80 in 1980[17]</v>
       </c>
       <c r="E84">
         <f>'UN Data'!B85</f>
@@ -70704,14 +70704,14 @@
       </c>
       <c r="B85">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C85" t="s">
         <v>490</v>
       </c>
       <c r="D85" t="str">
         <f t="shared" si="4"/>
-        <v>Population.Aged Over 80 in 1980[5]</v>
+        <v>Population.Aged Over 80 in 1980[16]</v>
       </c>
       <c r="E85">
         <f>'UN Data'!B86</f>
@@ -70724,14 +70724,14 @@
       </c>
       <c r="B86">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C86" t="s">
         <v>490</v>
       </c>
       <c r="D86" t="str">
         <f t="shared" si="4"/>
-        <v>Population.Aged Over 80 in 1980[6]</v>
+        <v>Population.Aged Over 80 in 1980[15]</v>
       </c>
       <c r="E86">
         <f>'UN Data'!B87</f>
@@ -70744,14 +70744,14 @@
       </c>
       <c r="B87">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C87" t="s">
         <v>490</v>
       </c>
       <c r="D87" t="str">
         <f t="shared" si="4"/>
-        <v>Population.Aged Over 80 in 1980[7]</v>
+        <v>Population.Aged Over 80 in 1980[14]</v>
       </c>
       <c r="E87">
         <f>'UN Data'!B88</f>
@@ -70764,14 +70764,14 @@
       </c>
       <c r="B88">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C88" t="s">
         <v>490</v>
       </c>
       <c r="D88" t="str">
         <f t="shared" si="4"/>
-        <v>Population.Aged Over 80 in 1980[8]</v>
+        <v>Population.Aged Over 80 in 1980[13]</v>
       </c>
       <c r="E88">
         <f>'UN Data'!B89</f>
@@ -70784,14 +70784,14 @@
       </c>
       <c r="B89">
         <f t="shared" si="3"/>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C89" t="s">
         <v>490</v>
       </c>
       <c r="D89" t="str">
         <f t="shared" si="4"/>
-        <v>Population.Aged Over 80 in 1980[9]</v>
+        <v>Population.Aged Over 80 in 1980[12]</v>
       </c>
       <c r="E89">
         <f>'UN Data'!B90</f>
@@ -70804,14 +70804,14 @@
       </c>
       <c r="B90">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C90" t="s">
         <v>490</v>
       </c>
       <c r="D90" t="str">
         <f t="shared" si="4"/>
-        <v>Population.Aged Over 80 in 1980[10]</v>
+        <v>Population.Aged Over 80 in 1980[11]</v>
       </c>
       <c r="E90">
         <f>'UN Data'!B91</f>
@@ -70824,14 +70824,14 @@
       </c>
       <c r="B91">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C91" t="s">
         <v>490</v>
       </c>
       <c r="D91" t="str">
         <f t="shared" si="4"/>
-        <v>Population.Aged Over 80 in 1980[11]</v>
+        <v>Population.Aged Over 80 in 1980[10]</v>
       </c>
       <c r="E91">
         <f>'UN Data'!B92</f>
@@ -70844,14 +70844,14 @@
       </c>
       <c r="B92">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C92" t="s">
         <v>490</v>
       </c>
       <c r="D92" t="str">
         <f t="shared" si="4"/>
-        <v>Population.Aged Over 80 in 1980[12]</v>
+        <v>Population.Aged Over 80 in 1980[9]</v>
       </c>
       <c r="E92">
         <f>'UN Data'!B93</f>
@@ -70864,14 +70864,14 @@
       </c>
       <c r="B93">
         <f t="shared" si="3"/>
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C93" t="s">
         <v>490</v>
       </c>
       <c r="D93" t="str">
         <f t="shared" si="4"/>
-        <v>Population.Aged Over 80 in 1980[13]</v>
+        <v>Population.Aged Over 80 in 1980[8]</v>
       </c>
       <c r="E93">
         <f>'UN Data'!B94</f>
@@ -70884,14 +70884,14 @@
       </c>
       <c r="B94">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C94" t="s">
         <v>490</v>
       </c>
       <c r="D94" t="str">
         <f t="shared" si="4"/>
-        <v>Population.Aged Over 80 in 1980[14]</v>
+        <v>Population.Aged Over 80 in 1980[7]</v>
       </c>
       <c r="E94">
         <f>'UN Data'!B95</f>
@@ -70904,14 +70904,14 @@
       </c>
       <c r="B95">
         <f t="shared" si="3"/>
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C95" t="s">
         <v>490</v>
       </c>
       <c r="D95" t="str">
         <f t="shared" si="4"/>
-        <v>Population.Aged Over 80 in 1980[15]</v>
+        <v>Population.Aged Over 80 in 1980[6]</v>
       </c>
       <c r="E95">
         <f>'UN Data'!B96</f>
@@ -70924,14 +70924,14 @@
       </c>
       <c r="B96">
         <f t="shared" si="3"/>
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C96" t="s">
         <v>490</v>
       </c>
       <c r="D96" t="str">
         <f t="shared" si="4"/>
-        <v>Population.Aged Over 80 in 1980[16]</v>
+        <v>Population.Aged Over 80 in 1980[5]</v>
       </c>
       <c r="E96">
         <f>'UN Data'!B97</f>
@@ -70944,14 +70944,14 @@
       </c>
       <c r="B97">
         <f t="shared" si="3"/>
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C97" t="s">
         <v>490</v>
       </c>
       <c r="D97" t="str">
         <f t="shared" si="4"/>
-        <v>Population.Aged Over 80 in 1980[17]</v>
+        <v>Population.Aged Over 80 in 1980[4]</v>
       </c>
       <c r="E97">
         <f>'UN Data'!B98</f>
@@ -70964,14 +70964,14 @@
       </c>
       <c r="B98">
         <f t="shared" si="3"/>
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="C98" t="s">
         <v>490</v>
       </c>
       <c r="D98" t="str">
         <f t="shared" si="4"/>
-        <v>Population.Aged Over 80 in 1980[18]</v>
+        <v>Population.Aged Over 80 in 1980[3]</v>
       </c>
       <c r="E98">
         <f>'UN Data'!B99</f>
@@ -70984,14 +70984,14 @@
       </c>
       <c r="B99">
         <f t="shared" si="3"/>
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="C99" t="s">
         <v>490</v>
       </c>
       <c r="D99" t="str">
         <f t="shared" si="4"/>
-        <v>Population.Aged Over 80 in 1980[19]</v>
+        <v>Population.Aged Over 80 in 1980[2]</v>
       </c>
       <c r="E99">
         <f>'UN Data'!B100</f>
@@ -71004,14 +71004,14 @@
       </c>
       <c r="B100">
         <f t="shared" si="3"/>
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C100" t="s">
         <v>490</v>
       </c>
       <c r="D100" t="str">
         <f t="shared" si="4"/>
-        <v>Population.Aged Over 80 in 1980[20]</v>
+        <v>Population.Aged Over 80 in 1980[1]</v>
       </c>
       <c r="E100">
         <f>'UN Data'!B101</f>
@@ -71059,7 +71059,7 @@
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>'Processing Initialization'!D2</f>
-        <v>Population.Aged 1 to 20 in 1980[1]</v>
+        <v>Population.Aged 1 to 20 in 1980[19]</v>
       </c>
       <c r="B2">
         <f>'Processing Initialization'!E2</f>
@@ -71077,7 +71077,7 @@
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f>'Processing Initialization'!D3</f>
-        <v>Population.Aged 1 to 20 in 1980[2]</v>
+        <v>Population.Aged 1 to 20 in 1980[18]</v>
       </c>
       <c r="B3">
         <f>'Processing Initialization'!E3</f>
@@ -71095,7 +71095,7 @@
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
         <f>'Processing Initialization'!D4</f>
-        <v>Population.Aged 1 to 20 in 1980[3]</v>
+        <v>Population.Aged 1 to 20 in 1980[17]</v>
       </c>
       <c r="B4">
         <f>'Processing Initialization'!E4</f>
@@ -71113,7 +71113,7 @@
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
         <f>'Processing Initialization'!D5</f>
-        <v>Population.Aged 1 to 20 in 1980[4]</v>
+        <v>Population.Aged 1 to 20 in 1980[16]</v>
       </c>
       <c r="B5">
         <f>'Processing Initialization'!E5</f>
@@ -71131,7 +71131,7 @@
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
         <f>'Processing Initialization'!D6</f>
-        <v>Population.Aged 1 to 20 in 1980[5]</v>
+        <v>Population.Aged 1 to 20 in 1980[15]</v>
       </c>
       <c r="B6">
         <f>'Processing Initialization'!E6</f>
@@ -71149,7 +71149,7 @@
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
         <f>'Processing Initialization'!D7</f>
-        <v>Population.Aged 1 to 20 in 1980[6]</v>
+        <v>Population.Aged 1 to 20 in 1980[14]</v>
       </c>
       <c r="B7">
         <f>'Processing Initialization'!E7</f>
@@ -71167,7 +71167,7 @@
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="str">
         <f>'Processing Initialization'!D8</f>
-        <v>Population.Aged 1 to 20 in 1980[7]</v>
+        <v>Population.Aged 1 to 20 in 1980[13]</v>
       </c>
       <c r="B8">
         <f>'Processing Initialization'!E8</f>
@@ -71185,7 +71185,7 @@
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="str">
         <f>'Processing Initialization'!D9</f>
-        <v>Population.Aged 1 to 20 in 1980[8]</v>
+        <v>Population.Aged 1 to 20 in 1980[12]</v>
       </c>
       <c r="B9">
         <f>'Processing Initialization'!E9</f>
@@ -71203,7 +71203,7 @@
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="str">
         <f>'Processing Initialization'!D10</f>
-        <v>Population.Aged 1 to 20 in 1980[9]</v>
+        <v>Population.Aged 1 to 20 in 1980[11]</v>
       </c>
       <c r="B10">
         <f>'Processing Initialization'!E10</f>
@@ -71239,7 +71239,7 @@
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="str">
         <f>'Processing Initialization'!D12</f>
-        <v>Population.Aged 1 to 20 in 1980[11]</v>
+        <v>Population.Aged 1 to 20 in 1980[9]</v>
       </c>
       <c r="B12">
         <f>'Processing Initialization'!E12</f>
@@ -71257,7 +71257,7 @@
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="str">
         <f>'Processing Initialization'!D13</f>
-        <v>Population.Aged 1 to 20 in 1980[12]</v>
+        <v>Population.Aged 1 to 20 in 1980[8]</v>
       </c>
       <c r="B13">
         <f>'Processing Initialization'!E13</f>
@@ -71275,7 +71275,7 @@
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="str">
         <f>'Processing Initialization'!D14</f>
-        <v>Population.Aged 1 to 20 in 1980[13]</v>
+        <v>Population.Aged 1 to 20 in 1980[7]</v>
       </c>
       <c r="B14">
         <f>'Processing Initialization'!E14</f>
@@ -71293,7 +71293,7 @@
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="str">
         <f>'Processing Initialization'!D15</f>
-        <v>Population.Aged 1 to 20 in 1980[14]</v>
+        <v>Population.Aged 1 to 20 in 1980[6]</v>
       </c>
       <c r="B15">
         <f>'Processing Initialization'!E15</f>
@@ -71311,7 +71311,7 @@
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="str">
         <f>'Processing Initialization'!D16</f>
-        <v>Population.Aged 1 to 20 in 1980[15]</v>
+        <v>Population.Aged 1 to 20 in 1980[5]</v>
       </c>
       <c r="B16">
         <f>'Processing Initialization'!E16</f>
@@ -71329,7 +71329,7 @@
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="str">
         <f>'Processing Initialization'!D17</f>
-        <v>Population.Aged 1 to 20 in 1980[16]</v>
+        <v>Population.Aged 1 to 20 in 1980[4]</v>
       </c>
       <c r="B17">
         <f>'Processing Initialization'!E17</f>
@@ -71347,7 +71347,7 @@
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="str">
         <f>'Processing Initialization'!D18</f>
-        <v>Population.Aged 1 to 20 in 1980[17]</v>
+        <v>Population.Aged 1 to 20 in 1980[3]</v>
       </c>
       <c r="B18">
         <f>'Processing Initialization'!E18</f>
@@ -71365,7 +71365,7 @@
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="str">
         <f>'Processing Initialization'!D19</f>
-        <v>Population.Aged 1 to 20 in 1980[18]</v>
+        <v>Population.Aged 1 to 20 in 1980[2]</v>
       </c>
       <c r="B19">
         <f>'Processing Initialization'!E19</f>
@@ -71383,7 +71383,7 @@
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="str">
         <f>'Processing Initialization'!D20</f>
-        <v>Population.Aged 1 to 20 in 1980[19]</v>
+        <v>Population.Aged 1 to 20 in 1980[1]</v>
       </c>
       <c r="B20">
         <f>'Processing Initialization'!E20</f>
@@ -71401,7 +71401,7 @@
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="str">
         <f>'Processing Initialization'!D21</f>
-        <v>Population.Aged 20 to 40 in 1980[1]</v>
+        <v>Population.Aged 20 to 40 in 1980[20]</v>
       </c>
       <c r="B21">
         <f>'Processing Initialization'!E21</f>
@@ -71419,7 +71419,7 @@
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="str">
         <f>'Processing Initialization'!D22</f>
-        <v>Population.Aged 20 to 40 in 1980[2]</v>
+        <v>Population.Aged 20 to 40 in 1980[19]</v>
       </c>
       <c r="B22">
         <f>'Processing Initialization'!E22</f>
@@ -71437,7 +71437,7 @@
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="str">
         <f>'Processing Initialization'!D23</f>
-        <v>Population.Aged 20 to 40 in 1980[3]</v>
+        <v>Population.Aged 20 to 40 in 1980[18]</v>
       </c>
       <c r="B23">
         <f>'Processing Initialization'!E23</f>
@@ -71455,7 +71455,7 @@
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="str">
         <f>'Processing Initialization'!D24</f>
-        <v>Population.Aged 20 to 40 in 1980[4]</v>
+        <v>Population.Aged 20 to 40 in 1980[17]</v>
       </c>
       <c r="B24">
         <f>'Processing Initialization'!E24</f>
@@ -71473,7 +71473,7 @@
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="str">
         <f>'Processing Initialization'!D25</f>
-        <v>Population.Aged 20 to 40 in 1980[5]</v>
+        <v>Population.Aged 20 to 40 in 1980[16]</v>
       </c>
       <c r="B25">
         <f>'Processing Initialization'!E25</f>
@@ -71491,7 +71491,7 @@
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="str">
         <f>'Processing Initialization'!D26</f>
-        <v>Population.Aged 20 to 40 in 1980[6]</v>
+        <v>Population.Aged 20 to 40 in 1980[15]</v>
       </c>
       <c r="B26">
         <f>'Processing Initialization'!E26</f>
@@ -71509,7 +71509,7 @@
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="str">
         <f>'Processing Initialization'!D27</f>
-        <v>Population.Aged 20 to 40 in 1980[7]</v>
+        <v>Population.Aged 20 to 40 in 1980[14]</v>
       </c>
       <c r="B27">
         <f>'Processing Initialization'!E27</f>
@@ -71527,7 +71527,7 @@
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="str">
         <f>'Processing Initialization'!D28</f>
-        <v>Population.Aged 20 to 40 in 1980[8]</v>
+        <v>Population.Aged 20 to 40 in 1980[13]</v>
       </c>
       <c r="B28">
         <f>'Processing Initialization'!E28</f>
@@ -71545,7 +71545,7 @@
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="str">
         <f>'Processing Initialization'!D29</f>
-        <v>Population.Aged 20 to 40 in 1980[9]</v>
+        <v>Population.Aged 20 to 40 in 1980[12]</v>
       </c>
       <c r="B29">
         <f>'Processing Initialization'!E29</f>
@@ -71563,7 +71563,7 @@
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="str">
         <f>'Processing Initialization'!D30</f>
-        <v>Population.Aged 20 to 40 in 1980[10]</v>
+        <v>Population.Aged 20 to 40 in 1980[11]</v>
       </c>
       <c r="B30">
         <f>'Processing Initialization'!E30</f>
@@ -71581,7 +71581,7 @@
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="str">
         <f>'Processing Initialization'!D31</f>
-        <v>Population.Aged 20 to 40 in 1980[11]</v>
+        <v>Population.Aged 20 to 40 in 1980[10]</v>
       </c>
       <c r="B31">
         <f>'Processing Initialization'!E31</f>
@@ -71599,7 +71599,7 @@
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="str">
         <f>'Processing Initialization'!D32</f>
-        <v>Population.Aged 20 to 40 in 1980[12]</v>
+        <v>Population.Aged 20 to 40 in 1980[9]</v>
       </c>
       <c r="B32">
         <f>'Processing Initialization'!E32</f>
@@ -71617,7 +71617,7 @@
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="str">
         <f>'Processing Initialization'!D33</f>
-        <v>Population.Aged 20 to 40 in 1980[13]</v>
+        <v>Population.Aged 20 to 40 in 1980[8]</v>
       </c>
       <c r="B33">
         <f>'Processing Initialization'!E33</f>
@@ -71635,7 +71635,7 @@
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="str">
         <f>'Processing Initialization'!D34</f>
-        <v>Population.Aged 20 to 40 in 1980[14]</v>
+        <v>Population.Aged 20 to 40 in 1980[7]</v>
       </c>
       <c r="B34">
         <f>'Processing Initialization'!E34</f>
@@ -71653,7 +71653,7 @@
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="str">
         <f>'Processing Initialization'!D35</f>
-        <v>Population.Aged 20 to 40 in 1980[15]</v>
+        <v>Population.Aged 20 to 40 in 1980[6]</v>
       </c>
       <c r="B35">
         <f>'Processing Initialization'!E35</f>
@@ -71671,7 +71671,7 @@
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="str">
         <f>'Processing Initialization'!D36</f>
-        <v>Population.Aged 20 to 40 in 1980[16]</v>
+        <v>Population.Aged 20 to 40 in 1980[5]</v>
       </c>
       <c r="B36">
         <f>'Processing Initialization'!E36</f>
@@ -71689,7 +71689,7 @@
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="str">
         <f>'Processing Initialization'!D37</f>
-        <v>Population.Aged 20 to 40 in 1980[17]</v>
+        <v>Population.Aged 20 to 40 in 1980[4]</v>
       </c>
       <c r="B37">
         <f>'Processing Initialization'!E37</f>
@@ -71707,7 +71707,7 @@
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="str">
         <f>'Processing Initialization'!D38</f>
-        <v>Population.Aged 20 to 40 in 1980[18]</v>
+        <v>Population.Aged 20 to 40 in 1980[3]</v>
       </c>
       <c r="B38">
         <f>'Processing Initialization'!E38</f>
@@ -71725,7 +71725,7 @@
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="str">
         <f>'Processing Initialization'!D39</f>
-        <v>Population.Aged 20 to 40 in 1980[19]</v>
+        <v>Population.Aged 20 to 40 in 1980[2]</v>
       </c>
       <c r="B39">
         <f>'Processing Initialization'!E39</f>
@@ -71743,7 +71743,7 @@
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="str">
         <f>'Processing Initialization'!D40</f>
-        <v>Population.Aged 20 to 40 in 1980[20]</v>
+        <v>Population.Aged 20 to 40 in 1980[1]</v>
       </c>
       <c r="B40">
         <f>'Processing Initialization'!E40</f>
@@ -71761,7 +71761,7 @@
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="str">
         <f>'Processing Initialization'!D41</f>
-        <v>Population.Aged 40 to 60 in 1980[1]</v>
+        <v>Population.Aged 40 to 60 in 1980[20]</v>
       </c>
       <c r="B41">
         <f>'Processing Initialization'!E41</f>
@@ -71779,7 +71779,7 @@
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="str">
         <f>'Processing Initialization'!D42</f>
-        <v>Population.Aged 40 to 60 in 1980[2]</v>
+        <v>Population.Aged 40 to 60 in 1980[19]</v>
       </c>
       <c r="B42">
         <f>'Processing Initialization'!E42</f>
@@ -71797,7 +71797,7 @@
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="str">
         <f>'Processing Initialization'!D43</f>
-        <v>Population.Aged 40 to 60 in 1980[3]</v>
+        <v>Population.Aged 40 to 60 in 1980[18]</v>
       </c>
       <c r="B43">
         <f>'Processing Initialization'!E43</f>
@@ -71815,7 +71815,7 @@
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="str">
         <f>'Processing Initialization'!D44</f>
-        <v>Population.Aged 40 to 60 in 1980[4]</v>
+        <v>Population.Aged 40 to 60 in 1980[17]</v>
       </c>
       <c r="B44">
         <f>'Processing Initialization'!E44</f>
@@ -71833,7 +71833,7 @@
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="str">
         <f>'Processing Initialization'!D45</f>
-        <v>Population.Aged 40 to 60 in 1980[5]</v>
+        <v>Population.Aged 40 to 60 in 1980[16]</v>
       </c>
       <c r="B45">
         <f>'Processing Initialization'!E45</f>
@@ -71851,7 +71851,7 @@
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="str">
         <f>'Processing Initialization'!D46</f>
-        <v>Population.Aged 40 to 60 in 1980[6]</v>
+        <v>Population.Aged 40 to 60 in 1980[15]</v>
       </c>
       <c r="B46">
         <f>'Processing Initialization'!E46</f>
@@ -71869,7 +71869,7 @@
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="str">
         <f>'Processing Initialization'!D47</f>
-        <v>Population.Aged 40 to 60 in 1980[7]</v>
+        <v>Population.Aged 40 to 60 in 1980[14]</v>
       </c>
       <c r="B47">
         <f>'Processing Initialization'!E47</f>
@@ -71887,7 +71887,7 @@
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="str">
         <f>'Processing Initialization'!D48</f>
-        <v>Population.Aged 40 to 60 in 1980[8]</v>
+        <v>Population.Aged 40 to 60 in 1980[13]</v>
       </c>
       <c r="B48">
         <f>'Processing Initialization'!E48</f>
@@ -71905,7 +71905,7 @@
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="str">
         <f>'Processing Initialization'!D49</f>
-        <v>Population.Aged 40 to 60 in 1980[9]</v>
+        <v>Population.Aged 40 to 60 in 1980[12]</v>
       </c>
       <c r="B49">
         <f>'Processing Initialization'!E49</f>
@@ -71923,7 +71923,7 @@
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="str">
         <f>'Processing Initialization'!D50</f>
-        <v>Population.Aged 40 to 60 in 1980[10]</v>
+        <v>Population.Aged 40 to 60 in 1980[11]</v>
       </c>
       <c r="B50">
         <f>'Processing Initialization'!E50</f>
@@ -71941,7 +71941,7 @@
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="str">
         <f>'Processing Initialization'!D51</f>
-        <v>Population.Aged 40 to 60 in 1980[11]</v>
+        <v>Population.Aged 40 to 60 in 1980[10]</v>
       </c>
       <c r="B51">
         <f>'Processing Initialization'!E51</f>
@@ -71959,7 +71959,7 @@
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="str">
         <f>'Processing Initialization'!D52</f>
-        <v>Population.Aged 40 to 60 in 1980[12]</v>
+        <v>Population.Aged 40 to 60 in 1980[9]</v>
       </c>
       <c r="B52">
         <f>'Processing Initialization'!E52</f>
@@ -71977,7 +71977,7 @@
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="str">
         <f>'Processing Initialization'!D53</f>
-        <v>Population.Aged 40 to 60 in 1980[13]</v>
+        <v>Population.Aged 40 to 60 in 1980[8]</v>
       </c>
       <c r="B53">
         <f>'Processing Initialization'!E53</f>
@@ -71995,7 +71995,7 @@
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="str">
         <f>'Processing Initialization'!D54</f>
-        <v>Population.Aged 40 to 60 in 1980[14]</v>
+        <v>Population.Aged 40 to 60 in 1980[7]</v>
       </c>
       <c r="B54">
         <f>'Processing Initialization'!E54</f>
@@ -72013,7 +72013,7 @@
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="str">
         <f>'Processing Initialization'!D55</f>
-        <v>Population.Aged 40 to 60 in 1980[15]</v>
+        <v>Population.Aged 40 to 60 in 1980[6]</v>
       </c>
       <c r="B55">
         <f>'Processing Initialization'!E55</f>
@@ -72031,7 +72031,7 @@
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="str">
         <f>'Processing Initialization'!D56</f>
-        <v>Population.Aged 40 to 60 in 1980[16]</v>
+        <v>Population.Aged 40 to 60 in 1980[5]</v>
       </c>
       <c r="B56">
         <f>'Processing Initialization'!E56</f>
@@ -72049,7 +72049,7 @@
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="str">
         <f>'Processing Initialization'!D57</f>
-        <v>Population.Aged 40 to 60 in 1980[17]</v>
+        <v>Population.Aged 40 to 60 in 1980[4]</v>
       </c>
       <c r="B57">
         <f>'Processing Initialization'!E57</f>
@@ -72067,7 +72067,7 @@
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="str">
         <f>'Processing Initialization'!D58</f>
-        <v>Population.Aged 40 to 60 in 1980[18]</v>
+        <v>Population.Aged 40 to 60 in 1980[3]</v>
       </c>
       <c r="B58">
         <f>'Processing Initialization'!E58</f>
@@ -72085,7 +72085,7 @@
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="str">
         <f>'Processing Initialization'!D59</f>
-        <v>Population.Aged 40 to 60 in 1980[19]</v>
+        <v>Population.Aged 40 to 60 in 1980[2]</v>
       </c>
       <c r="B59">
         <f>'Processing Initialization'!E59</f>
@@ -72103,7 +72103,7 @@
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="str">
         <f>'Processing Initialization'!D60</f>
-        <v>Population.Aged 40 to 60 in 1980[20]</v>
+        <v>Population.Aged 40 to 60 in 1980[1]</v>
       </c>
       <c r="B60">
         <f>'Processing Initialization'!E60</f>
@@ -72121,7 +72121,7 @@
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="str">
         <f>'Processing Initialization'!D61</f>
-        <v>Population.Aged 60 to 80 in 1980[1]</v>
+        <v>Population.Aged 60 to 80 in 1980[20]</v>
       </c>
       <c r="B61">
         <f>'Processing Initialization'!E61</f>
@@ -72139,7 +72139,7 @@
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="str">
         <f>'Processing Initialization'!D62</f>
-        <v>Population.Aged 60 to 80 in 1980[2]</v>
+        <v>Population.Aged 60 to 80 in 1980[19]</v>
       </c>
       <c r="B62">
         <f>'Processing Initialization'!E62</f>
@@ -72157,7 +72157,7 @@
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="str">
         <f>'Processing Initialization'!D63</f>
-        <v>Population.Aged 60 to 80 in 1980[3]</v>
+        <v>Population.Aged 60 to 80 in 1980[18]</v>
       </c>
       <c r="B63">
         <f>'Processing Initialization'!E63</f>
@@ -72175,7 +72175,7 @@
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="str">
         <f>'Processing Initialization'!D64</f>
-        <v>Population.Aged 60 to 80 in 1980[4]</v>
+        <v>Population.Aged 60 to 80 in 1980[17]</v>
       </c>
       <c r="B64">
         <f>'Processing Initialization'!E64</f>
@@ -72193,7 +72193,7 @@
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="str">
         <f>'Processing Initialization'!D65</f>
-        <v>Population.Aged 60 to 80 in 1980[5]</v>
+        <v>Population.Aged 60 to 80 in 1980[16]</v>
       </c>
       <c r="B65">
         <f>'Processing Initialization'!E65</f>
@@ -72211,7 +72211,7 @@
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="str">
         <f>'Processing Initialization'!D66</f>
-        <v>Population.Aged 60 to 80 in 1980[6]</v>
+        <v>Population.Aged 60 to 80 in 1980[15]</v>
       </c>
       <c r="B66">
         <f>'Processing Initialization'!E66</f>
@@ -72229,7 +72229,7 @@
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="str">
         <f>'Processing Initialization'!D67</f>
-        <v>Population.Aged 60 to 80 in 1980[7]</v>
+        <v>Population.Aged 60 to 80 in 1980[14]</v>
       </c>
       <c r="B67">
         <f>'Processing Initialization'!E67</f>
@@ -72247,7 +72247,7 @@
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="str">
         <f>'Processing Initialization'!D68</f>
-        <v>Population.Aged 60 to 80 in 1980[8]</v>
+        <v>Population.Aged 60 to 80 in 1980[13]</v>
       </c>
       <c r="B68">
         <f>'Processing Initialization'!E68</f>
@@ -72265,7 +72265,7 @@
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="str">
         <f>'Processing Initialization'!D69</f>
-        <v>Population.Aged 60 to 80 in 1980[9]</v>
+        <v>Population.Aged 60 to 80 in 1980[12]</v>
       </c>
       <c r="B69">
         <f>'Processing Initialization'!E69</f>
@@ -72283,7 +72283,7 @@
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="str">
         <f>'Processing Initialization'!D70</f>
-        <v>Population.Aged 60 to 80 in 1980[10]</v>
+        <v>Population.Aged 60 to 80 in 1980[11]</v>
       </c>
       <c r="B70">
         <f>'Processing Initialization'!E70</f>
@@ -72301,7 +72301,7 @@
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="str">
         <f>'Processing Initialization'!D71</f>
-        <v>Population.Aged 60 to 80 in 1980[11]</v>
+        <v>Population.Aged 60 to 80 in 1980[10]</v>
       </c>
       <c r="B71">
         <f>'Processing Initialization'!E71</f>
@@ -72319,7 +72319,7 @@
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="str">
         <f>'Processing Initialization'!D72</f>
-        <v>Population.Aged 60 to 80 in 1980[12]</v>
+        <v>Population.Aged 60 to 80 in 1980[9]</v>
       </c>
       <c r="B72">
         <f>'Processing Initialization'!E72</f>
@@ -72337,7 +72337,7 @@
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="str">
         <f>'Processing Initialization'!D73</f>
-        <v>Population.Aged 60 to 80 in 1980[13]</v>
+        <v>Population.Aged 60 to 80 in 1980[8]</v>
       </c>
       <c r="B73">
         <f>'Processing Initialization'!E73</f>
@@ -72355,7 +72355,7 @@
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="str">
         <f>'Processing Initialization'!D74</f>
-        <v>Population.Aged 60 to 80 in 1980[14]</v>
+        <v>Population.Aged 60 to 80 in 1980[7]</v>
       </c>
       <c r="B74">
         <f>'Processing Initialization'!E74</f>
@@ -72373,7 +72373,7 @@
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="str">
         <f>'Processing Initialization'!D75</f>
-        <v>Population.Aged 60 to 80 in 1980[15]</v>
+        <v>Population.Aged 60 to 80 in 1980[6]</v>
       </c>
       <c r="B75">
         <f>'Processing Initialization'!E75</f>
@@ -72391,7 +72391,7 @@
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="str">
         <f>'Processing Initialization'!D76</f>
-        <v>Population.Aged 60 to 80 in 1980[16]</v>
+        <v>Population.Aged 60 to 80 in 1980[5]</v>
       </c>
       <c r="B76">
         <f>'Processing Initialization'!E76</f>
@@ -72409,7 +72409,7 @@
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="str">
         <f>'Processing Initialization'!D77</f>
-        <v>Population.Aged 60 to 80 in 1980[17]</v>
+        <v>Population.Aged 60 to 80 in 1980[4]</v>
       </c>
       <c r="B77">
         <f>'Processing Initialization'!E77</f>
@@ -72427,7 +72427,7 @@
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="str">
         <f>'Processing Initialization'!D78</f>
-        <v>Population.Aged 60 to 80 in 1980[18]</v>
+        <v>Population.Aged 60 to 80 in 1980[3]</v>
       </c>
       <c r="B78">
         <f>'Processing Initialization'!E78</f>
@@ -72445,7 +72445,7 @@
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="str">
         <f>'Processing Initialization'!D79</f>
-        <v>Population.Aged 60 to 80 in 1980[19]</v>
+        <v>Population.Aged 60 to 80 in 1980[2]</v>
       </c>
       <c r="B79">
         <f>'Processing Initialization'!E79</f>
@@ -72463,7 +72463,7 @@
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="str">
         <f>'Processing Initialization'!D80</f>
-        <v>Population.Aged 60 to 80 in 1980[20]</v>
+        <v>Population.Aged 60 to 80 in 1980[1]</v>
       </c>
       <c r="B80">
         <f>'Processing Initialization'!E80</f>
@@ -72481,7 +72481,7 @@
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="str">
         <f>'Processing Initialization'!D81</f>
-        <v>Population.Aged Over 80 in 1980[1]</v>
+        <v>Population.Aged Over 80 in 1980[20]</v>
       </c>
       <c r="B81">
         <f>'Processing Initialization'!E81</f>
@@ -72499,7 +72499,7 @@
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="str">
         <f>'Processing Initialization'!D82</f>
-        <v>Population.Aged Over 80 in 1980[2]</v>
+        <v>Population.Aged Over 80 in 1980[19]</v>
       </c>
       <c r="B82">
         <f>'Processing Initialization'!E82</f>
@@ -72517,7 +72517,7 @@
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="str">
         <f>'Processing Initialization'!D83</f>
-        <v>Population.Aged Over 80 in 1980[3]</v>
+        <v>Population.Aged Over 80 in 1980[18]</v>
       </c>
       <c r="B83">
         <f>'Processing Initialization'!E83</f>
@@ -72535,7 +72535,7 @@
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="str">
         <f>'Processing Initialization'!D84</f>
-        <v>Population.Aged Over 80 in 1980[4]</v>
+        <v>Population.Aged Over 80 in 1980[17]</v>
       </c>
       <c r="B84">
         <f>'Processing Initialization'!E84</f>
@@ -72553,7 +72553,7 @@
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="str">
         <f>'Processing Initialization'!D85</f>
-        <v>Population.Aged Over 80 in 1980[5]</v>
+        <v>Population.Aged Over 80 in 1980[16]</v>
       </c>
       <c r="B85">
         <f>'Processing Initialization'!E85</f>
@@ -72571,7 +72571,7 @@
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" t="str">
         <f>'Processing Initialization'!D86</f>
-        <v>Population.Aged Over 80 in 1980[6]</v>
+        <v>Population.Aged Over 80 in 1980[15]</v>
       </c>
       <c r="B86">
         <f>'Processing Initialization'!E86</f>
@@ -72589,7 +72589,7 @@
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="str">
         <f>'Processing Initialization'!D87</f>
-        <v>Population.Aged Over 80 in 1980[7]</v>
+        <v>Population.Aged Over 80 in 1980[14]</v>
       </c>
       <c r="B87">
         <f>'Processing Initialization'!E87</f>
@@ -72607,7 +72607,7 @@
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="str">
         <f>'Processing Initialization'!D88</f>
-        <v>Population.Aged Over 80 in 1980[8]</v>
+        <v>Population.Aged Over 80 in 1980[13]</v>
       </c>
       <c r="B88">
         <f>'Processing Initialization'!E88</f>
@@ -72625,7 +72625,7 @@
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" t="str">
         <f>'Processing Initialization'!D89</f>
-        <v>Population.Aged Over 80 in 1980[9]</v>
+        <v>Population.Aged Over 80 in 1980[12]</v>
       </c>
       <c r="B89">
         <f>'Processing Initialization'!E89</f>
@@ -72643,7 +72643,7 @@
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="str">
         <f>'Processing Initialization'!D90</f>
-        <v>Population.Aged Over 80 in 1980[10]</v>
+        <v>Population.Aged Over 80 in 1980[11]</v>
       </c>
       <c r="B90">
         <f>'Processing Initialization'!E90</f>
@@ -72661,7 +72661,7 @@
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="str">
         <f>'Processing Initialization'!D91</f>
-        <v>Population.Aged Over 80 in 1980[11]</v>
+        <v>Population.Aged Over 80 in 1980[10]</v>
       </c>
       <c r="B91">
         <f>'Processing Initialization'!E91</f>
@@ -72679,7 +72679,7 @@
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="str">
         <f>'Processing Initialization'!D92</f>
-        <v>Population.Aged Over 80 in 1980[12]</v>
+        <v>Population.Aged Over 80 in 1980[9]</v>
       </c>
       <c r="B92">
         <f>'Processing Initialization'!E92</f>
@@ -72697,7 +72697,7 @@
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" t="str">
         <f>'Processing Initialization'!D93</f>
-        <v>Population.Aged Over 80 in 1980[13]</v>
+        <v>Population.Aged Over 80 in 1980[8]</v>
       </c>
       <c r="B93">
         <f>'Processing Initialization'!E93</f>
@@ -72715,7 +72715,7 @@
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="str">
         <f>'Processing Initialization'!D94</f>
-        <v>Population.Aged Over 80 in 1980[14]</v>
+        <v>Population.Aged Over 80 in 1980[7]</v>
       </c>
       <c r="B94">
         <f>'Processing Initialization'!E94</f>
@@ -72733,7 +72733,7 @@
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="str">
         <f>'Processing Initialization'!D95</f>
-        <v>Population.Aged Over 80 in 1980[15]</v>
+        <v>Population.Aged Over 80 in 1980[6]</v>
       </c>
       <c r="B95">
         <f>'Processing Initialization'!E95</f>
@@ -72751,7 +72751,7 @@
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="str">
         <f>'Processing Initialization'!D96</f>
-        <v>Population.Aged Over 80 in 1980[16]</v>
+        <v>Population.Aged Over 80 in 1980[5]</v>
       </c>
       <c r="B96">
         <f>'Processing Initialization'!E96</f>
@@ -72769,7 +72769,7 @@
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="str">
         <f>'Processing Initialization'!D97</f>
-        <v>Population.Aged Over 80 in 1980[17]</v>
+        <v>Population.Aged Over 80 in 1980[4]</v>
       </c>
       <c r="B97">
         <f>'Processing Initialization'!E97</f>
@@ -72787,7 +72787,7 @@
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="str">
         <f>'Processing Initialization'!D98</f>
-        <v>Population.Aged Over 80 in 1980[18]</v>
+        <v>Population.Aged Over 80 in 1980[3]</v>
       </c>
       <c r="B98">
         <f>'Processing Initialization'!E98</f>
@@ -72805,7 +72805,7 @@
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="str">
         <f>'Processing Initialization'!D99</f>
-        <v>Population.Aged Over 80 in 1980[19]</v>
+        <v>Population.Aged Over 80 in 1980[2]</v>
       </c>
       <c r="B99">
         <f>'Processing Initialization'!E99</f>
@@ -72823,7 +72823,7 @@
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="str">
         <f>'Processing Initialization'!D100</f>
-        <v>Population.Aged Over 80 in 1980[20]</v>
+        <v>Population.Aged Over 80 in 1980[1]</v>
       </c>
       <c r="B100">
         <f>'Processing Initialization'!E100</f>
@@ -72847,7 +72847,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E25B45F-292B-A645-8C83-09B23CAEE818}">
   <dimension ref="A1:AT17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>

</xml_diff>